<commit_message>
CSS fixed on different pages
</commit_message>
<xml_diff>
--- a/misc/relationalTableDraftOne.xlsx
+++ b/misc/relationalTableDraftOne.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\max.KORENVAES\CodingBootcamp\Project2-Group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TONRIN\Project2-Group2\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4D7516B-6798-404B-AAFE-EA7C0A29D71D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80430E5-93D1-4A13-83D9-FF513905F10A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{DE93122A-39FD-43C1-B58C-913B640B1595}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{DE93122A-39FD-43C1-B58C-913B640B1595}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
   <si>
     <t>ToyName</t>
   </si>
@@ -156,13 +150,37 @@
     <t>TableName: Users, TableFrom: User Signup</t>
   </si>
   <si>
-    <t>TableName: Inventory, From: Managers&amp;Users via Orders</t>
-  </si>
-  <si>
     <t>Orders, Inventory</t>
   </si>
   <si>
     <t>ToyID</t>
+  </si>
+  <si>
+    <t>TableName: Toys, From: Managers&amp;Users via Orders</t>
+  </si>
+  <si>
+    <t>ToyRating</t>
+  </si>
+  <si>
+    <t>Age Limit</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>Solitaire</t>
+  </si>
+  <si>
+    <t>Team Play</t>
   </si>
 </sst>
 </file>
@@ -559,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E226B4-7500-47E5-9915-4F1F8DA11008}">
-  <dimension ref="B6:P25"/>
+  <dimension ref="B6:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1079,7 @@
         <v>22</v>
       </c>
       <c r="P18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1086,7 +1104,7 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1114,7 +1132,7 @@
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1179,6 +1197,75 @@
       </c>
       <c r="H25" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>